<commit_message>
data-driven admin login test
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsfile/data.xlsx
+++ b/src/main/resources/xlsfile/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051219B1-B53D-464D-A3D3-CFBC5461FEAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE6AF8-1AA4-0846-BDE9-BAB305ED7E56}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="3" r:id="rId1"/>
@@ -258,8 +258,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A61EC612-364F-4AAF-854A-8EA0A5A8A249}" name="Table1" displayName="Table1" ref="B2:D5" totalsRowShown="0">
-  <autoFilter ref="B2:D5" xr:uid="{62AEE2EB-9312-477C-9ABE-7CBF8BA419AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A61EC612-364F-4AAF-854A-8EA0A5A8A249}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{62AEE2EB-9312-477C-9ABE-7CBF8BA419AF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BA57E4BE-7DBA-485B-8830-0456D412F42A}" name="username"/>
     <tableColumn id="2" xr3:uid="{E8000F9C-05B2-4F8C-B276-8A582504A7C7}" name="password"/>
@@ -270,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D25E7CD-EFAA-455E-A8C0-3DAF6CF94C9B}" name="Table2" displayName="Table2" ref="B2:F8" totalsRowShown="0">
-  <autoFilter ref="B2:F8" xr:uid="{E88A2A4A-0552-46F7-B801-575480B4D623}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D25E7CD-EFAA-455E-A8C0-3DAF6CF94C9B}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7" xr:uid="{E88A2A4A-0552-46F7-B801-575480B4D623}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4234200A-24A3-4431-96E4-64948AB97A1B}" name="productId"/>
     <tableColumn id="2" xr3:uid="{85BFE5BF-A718-4639-B784-3A9E3DF9453C}" name="name"/>
@@ -284,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49A3D75E-4310-44D5-972B-2640E3A4E08D}" name="Table3" displayName="Table3" ref="B2:D8" totalsRowShown="0">
-  <autoFilter ref="B2:D8" xr:uid="{3BDDC653-3007-4EE7-9940-1CFE364DAB20}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49A3D75E-4310-44D5-972B-2640E3A4E08D}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{3BDDC653-3007-4EE7-9940-1CFE364DAB20}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C9115DC6-00C1-4B86-9CF3-1569B48BAE07}" name="transactionId"/>
     <tableColumn id="2" xr3:uid="{562F3536-BAC0-402A-9AE6-60CAC9D89960}" name="ProductId"/>
@@ -558,59 +558,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1026DCF3-1AA9-47CE-A1A2-F3A87C93FA91}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -624,137 +624,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B2F33-3E03-494D-9F30-1DF0D32D4E4D}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="E7" s="1">
         <v>-1</v>
       </c>
     </row>
@@ -769,93 +769,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
       <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
       <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8">
+      <c r="C7">
         <v>6</v>
       </c>
     </row>
@@ -869,38 +869,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5A8D0-6A69-4317-BF67-BDCA8742CFBC}">
-  <dimension ref="B2:C4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
       <c r="B3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
restore original Excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsfile/data.xlsx
+++ b/src/main/resources/xlsfile/data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE6AF8-1AA4-0846-BDE9-BAB305ED7E56}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051219B1-B53D-464D-A3D3-CFBC5461FEAC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="22260" windowHeight="12640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="3" r:id="rId1"/>
@@ -258,8 +258,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A61EC612-364F-4AAF-854A-8EA0A5A8A249}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{62AEE2EB-9312-477C-9ABE-7CBF8BA419AF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A61EC612-364F-4AAF-854A-8EA0A5A8A249}" name="Table1" displayName="Table1" ref="B2:D5" totalsRowShown="0">
+  <autoFilter ref="B2:D5" xr:uid="{62AEE2EB-9312-477C-9ABE-7CBF8BA419AF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BA57E4BE-7DBA-485B-8830-0456D412F42A}" name="username"/>
     <tableColumn id="2" xr3:uid="{E8000F9C-05B2-4F8C-B276-8A582504A7C7}" name="password"/>
@@ -270,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D25E7CD-EFAA-455E-A8C0-3DAF6CF94C9B}" name="Table2" displayName="Table2" ref="A1:E7" totalsRowShown="0">
-  <autoFilter ref="A1:E7" xr:uid="{E88A2A4A-0552-46F7-B801-575480B4D623}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D25E7CD-EFAA-455E-A8C0-3DAF6CF94C9B}" name="Table2" displayName="Table2" ref="B2:F8" totalsRowShown="0">
+  <autoFilter ref="B2:F8" xr:uid="{E88A2A4A-0552-46F7-B801-575480B4D623}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{4234200A-24A3-4431-96E4-64948AB97A1B}" name="productId"/>
     <tableColumn id="2" xr3:uid="{85BFE5BF-A718-4639-B784-3A9E3DF9453C}" name="name"/>
@@ -284,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49A3D75E-4310-44D5-972B-2640E3A4E08D}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{3BDDC653-3007-4EE7-9940-1CFE364DAB20}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{49A3D75E-4310-44D5-972B-2640E3A4E08D}" name="Table3" displayName="Table3" ref="B2:D8" totalsRowShown="0">
+  <autoFilter ref="B2:D8" xr:uid="{3BDDC653-3007-4EE7-9940-1CFE364DAB20}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C9115DC6-00C1-4B86-9CF3-1569B48BAE07}" name="transactionId"/>
     <tableColumn id="2" xr3:uid="{562F3536-BAC0-402A-9AE6-60CAC9D89960}" name="ProductId"/>
@@ -558,59 +558,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1026DCF3-1AA9-47CE-A1A2-F3A87C93FA91}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -624,137 +624,137 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{077B2F33-3E03-494D-9F30-1DF0D32D4E4D}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F3" s="1">
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F4" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F5" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F6" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F7" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F8" s="1">
         <v>-1</v>
       </c>
     </row>
@@ -769,93 +769,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="D4">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="D7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <v>6</v>
       </c>
     </row>
@@ -869,38 +869,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D5A8D0-6A69-4317-BF67-BDCA8742CFBC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>